<commit_message>
Updated the Burndown chart
Didn't get much work done because I ran into a bug with parcelable and Serializable object, but it works now.
</commit_message>
<xml_diff>
--- a/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
+++ b/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Git\BehrmanCSE248\_FinalPlanning\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1793D2DA-ED17-422C-B1B0-9F65F5BE5D21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33E9588-C2C3-4D7F-B651-3BCD1C72C51C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{2B62D9C2-9DC6-4999-B35D-877F52857D40}"/>
   </bookViews>
@@ -86,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -186,80 +186,71 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +569,7 @@
   <dimension ref="B3:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,237 +578,247 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="1">
         <v>43399</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="10">
         <v>2</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="10">
         <v>5</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="10">
         <v>8</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="2">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="10">
         <v>10</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="G13" s="2">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="24">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="14">
         <f>SUM(F5:F14)</f>
         <v>27</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="14">
         <f t="shared" ref="G15:K15" si="0">SUM(G5:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="24">
+        <v>26</v>
+      </c>
+      <c r="H15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="50">
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
@@ -825,13 +826,15 @@
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="K17:K18"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
     <mergeCell ref="B15:E16"/>
     <mergeCell ref="B17:E18"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="B13:E14"/>
     <mergeCell ref="B11:E12"/>
     <mergeCell ref="F5:F6"/>
@@ -843,6 +846,29 @@
     <mergeCell ref="B5:E6"/>
     <mergeCell ref="B7:E8"/>
     <mergeCell ref="B9:E10"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the burndown chart for 10/27/18. The View History feature is taking longer than expected. Reached breakthrough last night. Just need to configure some layouts
</commit_message>
<xml_diff>
--- a/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
+++ b/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Git\BehrmanCSE248\_FinalPlanning\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33E9588-C2C3-4D7F-B651-3BCD1C72C51C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B3E70-BF54-4A98-AC1D-3639E8141BAF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{2B62D9C2-9DC6-4999-B35D-877F52857D40}"/>
   </bookViews>
@@ -204,53 +204,53 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,256 +569,310 @@
   <dimension ref="B3:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>43399</v>
       </c>
+      <c r="H3" s="1">
+        <v>43400</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="10">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="15">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8">
+        <v>5</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="10">
+      <c r="G7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="8">
         <v>2</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="10">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="15">
         <v>5</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="8">
         <v>5</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="H9" s="8">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="10">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="15">
         <v>8</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="8">
         <v>8</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="H11" s="8">
+        <v>8</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="10">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="15">
         <v>10</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="8">
         <v>10</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="H13" s="8">
+        <v>10</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="2">
         <f>SUM(F5:F14)</f>
-        <v>27</v>
-      </c>
-      <c r="G15" s="14">
+        <v>35</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" ref="G15:K15" si="0">SUM(G5:G14)</f>
-        <v>26</v>
-      </c>
-      <c r="H15" s="14">
+        <v>32</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="14">
+      <c r="J15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="14">
+      <c r="K15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B13:E14"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
@@ -828,47 +882,6 @@
     <mergeCell ref="K17:K18"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="B17:E18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B13:E14"/>
-    <mergeCell ref="B11:E12"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Manual Transactions Pretty Much Complete Just need a edit manual transactions and we'll be set. With that, the project is almost finish. Some things to work on: 1. Layout (Mainly menu) 2. Webhook for transactions with plaid 3. Add Strings to strings.xml 4. Clean up code in all classes 5. Change LinkedList to ArrayList for the Transaction Parsers 6. Add a ListView layout for the view transactions history with the calendar view. 7. Add some sort of calculator to calculate how much was spent each month. 8. Query for transactions on a card (would be hard to do on a auto card) 9. Have all network calls be on the server (main.js cloud functions) 10. Update UML Charts 11. Update Burn down chart and create graph
</commit_message>
<xml_diff>
--- a/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
+++ b/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Git\BehrmanCSE248\_FinalPlanning\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6207B36E-B2F5-4C5C-8D3B-3C022518ECAE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE10CA84-E0DA-45AB-B634-463DAE67A115}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{2B62D9C2-9DC6-4999-B35D-877F52857D40}"/>
   </bookViews>
@@ -30,15 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tasks</t>
   </si>
   <si>
     <t>Points</t>
-  </si>
-  <si>
-    <t>View History Activies</t>
   </si>
   <si>
     <t>Edit Cards</t>
@@ -57,6 +54,12 @@
   </si>
   <si>
     <t>Estimated</t>
+  </si>
+  <si>
+    <t>View History Activities</t>
+  </si>
+  <si>
+    <t>Add Manual Transaction</t>
   </si>
 </sst>
 </file>
@@ -204,53 +207,53 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,24 +569,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561CFD15-C30D-40CC-AF2A-0CE4DF52F7FE}">
-  <dimension ref="B3:K18"/>
+  <dimension ref="B3:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J16"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" t="s">
         <v>1</v>
       </c>
@@ -596,57 +599,65 @@
       <c r="I3" s="1">
         <v>43402</v>
       </c>
+      <c r="J3" s="1">
+        <v>43403</v>
+      </c>
+      <c r="K3" s="1">
+        <v>43404</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="15">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8">
+        <v>5</v>
+      </c>
+      <c r="I5" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="10">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="J5" s="8">
         <v>2</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="8">
         <v>2</v>
       </c>
-      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="10">
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="15">
         <v>3</v>
       </c>
       <c r="G7" s="2">
@@ -659,252 +670,305 @@
         <v>3</v>
       </c>
       <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="15">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
+        <v>3</v>
+      </c>
+      <c r="I9" s="8">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="15">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5</v>
+      </c>
+      <c r="H11" s="8">
+        <v>5</v>
+      </c>
+      <c r="I11" s="8">
+        <v>5</v>
+      </c>
+      <c r="J11" s="8">
+        <v>5</v>
+      </c>
+      <c r="K11" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="10">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="15">
+        <v>8</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8</v>
+      </c>
+      <c r="H13" s="8">
+        <v>8</v>
+      </c>
+      <c r="I13" s="8">
+        <v>8</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2">
-        <v>5</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5</v>
-      </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="10">
-        <v>8</v>
-      </c>
-      <c r="G11" s="2">
-        <v>8</v>
-      </c>
-      <c r="H11" s="2">
-        <v>8</v>
-      </c>
-      <c r="I11" s="2">
-        <v>8</v>
-      </c>
-      <c r="J11" s="2">
-        <v>8</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="10">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="15">
         <v>10</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G15" s="8">
         <v>10</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H15" s="8">
         <v>10</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I15" s="8">
         <v>10</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J15" s="8">
         <v>10</v>
       </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14">
-        <f>SUM(F5:F14)</f>
-        <v>36</v>
-      </c>
-      <c r="G15" s="14">
-        <f t="shared" ref="G15:K15" si="0">SUM(G5:G14)</f>
-        <v>33</v>
-      </c>
-      <c r="H15" s="14">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="I15" s="14">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="J15" s="14">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="K15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K15" s="8">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="2">
+        <f>SUM(F5:F16)</f>
+        <v>39</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(G5:G16)</f>
+        <v>36</v>
+      </c>
+      <c r="H17" s="2">
+        <f>SUM(H5:H16)</f>
+        <v>34</v>
+      </c>
+      <c r="I17" s="2">
+        <f>SUM(I5:I16)</f>
+        <v>31</v>
+      </c>
+      <c r="J17" s="2">
+        <f>SUM(J5:J16)</f>
+        <v>29</v>
+      </c>
+      <c r="K17" s="2">
+        <f>SUM(K5:K16)</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="57">
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
     <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="B13:E14"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="B19:E20"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="B17:E18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B13:E14"/>
-    <mergeCell ref="B11:E12"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Burndown Chart Fixed the padding on some layouts and updated the burndown chart. I keep needing to add more points to features because they were taking longer than expected. This is starting to become more of a burnup chart I think. I need to start working on the uml diagrams in more detail and make some more diagrams for the project for the demo when this project is due.
</commit_message>
<xml_diff>
--- a/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
+++ b/_FinalPlanning/BurnDown/Burn Down Chart Draft.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Git\BehrmanCSE248\_FinalPlanning\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89CA563-BB6F-4255-8B21-1EE83AFDAAC0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1C180E-47EB-4D5D-B0FC-8468AADB1760}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{2B62D9C2-9DC6-4999-B35D-877F52857D40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Tasks</t>
   </si>
@@ -65,9 +66,6 @@
     <t>View Monthly Payment History</t>
   </si>
   <si>
-    <t>(!)</t>
-  </si>
-  <si>
     <t>Connection Fail Handling</t>
   </si>
   <si>
@@ -75,6 +73,9 @@
   </si>
   <si>
     <t>Querying Transactions</t>
+  </si>
+  <si>
+    <t>(!) Lot done</t>
   </si>
 </sst>
 </file>
@@ -226,19 +227,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,7 +588,7 @@
   <dimension ref="B3:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9:O10"/>
+      <selection activeCell="O5" sqref="O5:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +642,7 @@
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="N4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -652,33 +653,33 @@
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="14">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5">
         <v>17</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="5">
         <v>15</v>
       </c>
-      <c r="H5" s="7">
-        <v>13</v>
-      </c>
-      <c r="I5" s="7">
-        <v>10</v>
-      </c>
-      <c r="J5" s="7">
-        <v>10</v>
-      </c>
-      <c r="K5" s="7">
-        <v>10</v>
-      </c>
-      <c r="L5" s="7">
-        <v>5</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7">
+      <c r="I5" s="5">
+        <v>12</v>
+      </c>
+      <c r="J5" s="5">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5">
+        <v>12</v>
+      </c>
+      <c r="L5" s="5">
+        <v>7</v>
+      </c>
+      <c r="M5" s="5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -688,15 +689,15 @@
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -708,31 +709,31 @@
       <c r="F7" s="14">
         <v>3</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>3</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>3</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <v>3</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <v>3</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -742,15 +743,15 @@
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -762,31 +763,31 @@
       <c r="F9" s="14">
         <v>3</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>3</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>3</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <v>3</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="5">
         <v>1</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="5">
         <v>1</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="5">
         <v>1</v>
       </c>
-      <c r="N9" s="7">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7">
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -796,15 +797,15 @@
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
@@ -816,31 +817,31 @@
       <c r="F11" s="14">
         <v>5</v>
       </c>
-      <c r="G11" s="7">
-        <v>5</v>
-      </c>
-      <c r="H11" s="7">
-        <v>5</v>
-      </c>
-      <c r="I11" s="7">
-        <v>5</v>
-      </c>
-      <c r="J11" s="7">
-        <v>5</v>
-      </c>
-      <c r="K11" s="7">
-        <v>5</v>
-      </c>
-      <c r="L11" s="7">
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5">
+        <v>5</v>
+      </c>
+      <c r="K11" s="5">
+        <v>5</v>
+      </c>
+      <c r="L11" s="5">
         <v>4</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="5">
         <v>1</v>
       </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
         <v>0</v>
       </c>
     </row>
@@ -850,15 +851,15 @@
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
@@ -868,33 +869,33 @@
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="14">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5">
+        <v>10</v>
+      </c>
+      <c r="I13" s="5">
+        <v>10</v>
+      </c>
+      <c r="J13" s="5">
+        <v>10</v>
+      </c>
+      <c r="K13" s="5">
+        <v>10</v>
+      </c>
+      <c r="L13" s="5">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5">
         <v>8</v>
       </c>
-      <c r="G13" s="7">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7">
-        <v>8</v>
-      </c>
-      <c r="I13" s="7">
-        <v>8</v>
-      </c>
-      <c r="J13" s="7">
-        <v>8</v>
-      </c>
-      <c r="K13" s="7">
-        <v>8</v>
-      </c>
-      <c r="L13" s="7">
-        <v>8</v>
-      </c>
-      <c r="M13" s="7">
-        <v>7</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
+      <c r="N13" s="5">
+        <v>2</v>
+      </c>
+      <c r="O13" s="5">
         <v>0</v>
       </c>
     </row>
@@ -904,15 +905,15 @@
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -924,31 +925,31 @@
       <c r="F15" s="14">
         <v>5</v>
       </c>
-      <c r="G15" s="5">
-        <v>5</v>
-      </c>
-      <c r="H15" s="5">
-        <v>5</v>
-      </c>
-      <c r="I15" s="5">
-        <v>5</v>
-      </c>
-      <c r="J15" s="5">
-        <v>5</v>
-      </c>
-      <c r="K15" s="5">
-        <v>5</v>
-      </c>
-      <c r="L15" s="5">
-        <v>5</v>
-      </c>
-      <c r="M15" s="5">
-        <v>5</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>5</v>
+      </c>
+      <c r="I15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3">
+        <v>5</v>
+      </c>
+      <c r="K15" s="3">
+        <v>5</v>
+      </c>
+      <c r="L15" s="3">
+        <v>5</v>
+      </c>
+      <c r="M15" s="3">
+        <v>5</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -958,19 +959,19 @@
       <c r="D16" s="12"/>
       <c r="E16" s="13"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -978,31 +979,31 @@
       <c r="F17" s="14">
         <v>7</v>
       </c>
-      <c r="G17" s="5">
-        <v>7</v>
-      </c>
-      <c r="H17" s="5">
-        <v>7</v>
-      </c>
-      <c r="I17" s="5">
-        <v>7</v>
-      </c>
-      <c r="J17" s="5">
-        <v>7</v>
-      </c>
-      <c r="K17" s="5">
-        <v>7</v>
-      </c>
-      <c r="L17" s="5">
-        <v>7</v>
-      </c>
-      <c r="M17" s="5">
-        <v>7</v>
-      </c>
-      <c r="N17" s="5">
-        <v>7</v>
-      </c>
-      <c r="O17" s="5">
+      <c r="G17" s="3">
+        <v>7</v>
+      </c>
+      <c r="H17" s="3">
+        <v>7</v>
+      </c>
+      <c r="I17" s="3">
+        <v>7</v>
+      </c>
+      <c r="J17" s="3">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3">
+        <v>7</v>
+      </c>
+      <c r="L17" s="3">
+        <v>7</v>
+      </c>
+      <c r="M17" s="3">
+        <v>7</v>
+      </c>
+      <c r="N17" s="3">
+        <v>7</v>
+      </c>
+      <c r="O17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1012,19 +1013,19 @@
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1032,31 +1033,31 @@
       <c r="F19" s="14">
         <v>7</v>
       </c>
-      <c r="G19" s="5">
-        <v>7</v>
-      </c>
-      <c r="H19" s="5">
-        <v>7</v>
-      </c>
-      <c r="I19" s="5">
-        <v>7</v>
-      </c>
-      <c r="J19" s="5">
-        <v>7</v>
-      </c>
-      <c r="K19" s="5">
-        <v>7</v>
-      </c>
-      <c r="L19" s="5">
-        <v>7</v>
-      </c>
-      <c r="M19" s="5">
-        <v>7</v>
-      </c>
-      <c r="N19" s="5">
-        <v>7</v>
-      </c>
-      <c r="O19" s="5">
+      <c r="G19" s="3">
+        <v>7</v>
+      </c>
+      <c r="H19" s="3">
+        <v>7</v>
+      </c>
+      <c r="I19" s="3">
+        <v>7</v>
+      </c>
+      <c r="J19" s="3">
+        <v>7</v>
+      </c>
+      <c r="K19" s="3">
+        <v>7</v>
+      </c>
+      <c r="L19" s="3">
+        <v>7</v>
+      </c>
+      <c r="M19" s="3">
+        <v>7</v>
+      </c>
+      <c r="N19" s="3">
+        <v>7</v>
+      </c>
+      <c r="O19" s="3">
         <v>7</v>
       </c>
     </row>
@@ -1066,19 +1067,19 @@
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1086,31 +1087,31 @@
       <c r="F21" s="14">
         <v>5</v>
       </c>
-      <c r="G21" s="5">
-        <v>5</v>
-      </c>
-      <c r="H21" s="5">
-        <v>5</v>
-      </c>
-      <c r="I21" s="5">
-        <v>5</v>
-      </c>
-      <c r="J21" s="5">
-        <v>5</v>
-      </c>
-      <c r="K21" s="5">
-        <v>5</v>
-      </c>
-      <c r="L21" s="5">
-        <v>5</v>
-      </c>
-      <c r="M21" s="5">
-        <v>5</v>
-      </c>
-      <c r="N21" s="5">
-        <v>5</v>
-      </c>
-      <c r="O21" s="5">
+      <c r="G21" s="3">
+        <v>5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>5</v>
+      </c>
+      <c r="J21" s="3">
+        <v>5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>5</v>
+      </c>
+      <c r="L21" s="3">
+        <v>5</v>
+      </c>
+      <c r="M21" s="3">
+        <v>5</v>
+      </c>
+      <c r="N21" s="3">
+        <v>5</v>
+      </c>
+      <c r="O21" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1120,15 +1121,15 @@
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
@@ -1140,31 +1141,31 @@
       <c r="F23" s="14">
         <v>10</v>
       </c>
-      <c r="G23" s="7">
-        <v>10</v>
-      </c>
-      <c r="H23" s="7">
-        <v>10</v>
-      </c>
-      <c r="I23" s="7">
-        <v>10</v>
-      </c>
-      <c r="J23" s="7">
-        <v>10</v>
-      </c>
-      <c r="K23" s="7">
-        <v>10</v>
-      </c>
-      <c r="L23" s="7">
-        <v>10</v>
-      </c>
-      <c r="M23" s="7">
-        <v>10</v>
-      </c>
-      <c r="N23" s="7">
-        <v>0</v>
-      </c>
-      <c r="O23" s="7">
+      <c r="G23" s="5">
+        <v>10</v>
+      </c>
+      <c r="H23" s="5">
+        <v>10</v>
+      </c>
+      <c r="I23" s="5">
+        <v>10</v>
+      </c>
+      <c r="J23" s="5">
+        <v>10</v>
+      </c>
+      <c r="K23" s="5">
+        <v>10</v>
+      </c>
+      <c r="L23" s="5">
+        <v>10</v>
+      </c>
+      <c r="M23" s="5">
+        <v>10</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+      <c r="O23" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1174,15 +1175,15 @@
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
@@ -1191,42 +1192,42 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="5">
+      <c r="F25" s="3">
         <f>SUM(F5:F24)</f>
+        <v>75</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" ref="G25:L25" si="0">SUM(G5:G24)</f>
+        <v>72</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="G25" s="5">
-        <f>SUM(G5:G24)</f>
-        <v>68</v>
-      </c>
-      <c r="H25" s="5">
-        <f>SUM(H5:H24)</f>
-        <v>66</v>
-      </c>
-      <c r="I25" s="5">
-        <f>SUM(I5:I24)</f>
-        <v>63</v>
-      </c>
-      <c r="J25" s="5">
-        <f>SUM(J5:J24)</f>
-        <v>61</v>
-      </c>
-      <c r="K25" s="5">
-        <f>SUM(K5:K24)</f>
-        <v>61</v>
-      </c>
-      <c r="L25" s="5">
-        <f>SUM(L5:L24)</f>
-        <v>53</v>
-      </c>
-      <c r="M25" s="5">
-        <v>0</v>
-      </c>
-      <c r="N25" s="5">
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
         <f>SUM(N5:N24)</f>
-        <v>19</v>
-      </c>
-      <c r="O25" s="5">
+        <v>24</v>
+      </c>
+      <c r="O25" s="3">
         <f>SUM(O5:O24)</f>
         <v>10</v>
       </c>
@@ -1236,16 +1237,16 @@
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
@@ -1254,44 +1255,44 @@
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="3">
+      <c r="F27" s="6">
         <f>SUM(F5:F23)</f>
+        <v>75</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" ref="G27:O27" si="1">SUM(G5:G23)</f>
+        <v>72</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="G27" s="3">
-        <f>SUM(G5:G23)</f>
-        <v>68</v>
-      </c>
-      <c r="H27" s="3">
-        <f>SUM(H5:H23)</f>
-        <v>66</v>
-      </c>
-      <c r="I27" s="3">
-        <f>SUM(I5:I23)</f>
-        <v>63</v>
-      </c>
-      <c r="J27" s="3">
-        <f>SUM(J5:J23)</f>
-        <v>61</v>
-      </c>
-      <c r="K27" s="3">
-        <f>SUM(K5:K23)</f>
-        <v>61</v>
-      </c>
-      <c r="L27" s="3">
-        <f>SUM(L5:L23)</f>
-        <v>53</v>
-      </c>
-      <c r="M27" s="3">
-        <f>SUM(M5:M23)</f>
-        <v>44</v>
-      </c>
-      <c r="N27" s="3">
-        <f>SUM(N5:N23)</f>
-        <v>19</v>
-      </c>
-      <c r="O27" s="3">
-        <f>SUM(O5:O23)</f>
+      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="M27" s="6">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="N27" s="6">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -1300,72 +1301,69 @@
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="133">
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B17:E18"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="H11:H12"/>
@@ -1390,62 +1388,65 @@
     <mergeCell ref="B13:E14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="B25:E26"/>
     <mergeCell ref="B27:E28"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="K25:K26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>